<commit_message>
enh: update plies written
</commit_message>
<xml_diff>
--- a/wing_optimization_SSSS/loads/evolution.xlsx
+++ b/wing_optimization_SSSS/loads/evolution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rafael-Documentos-trabalhos\PERIODOS\ITA-2019--\0 - TESE\_works\box_structural_optimization\11th trial\loads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\wing_optimization_SSSS\loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B21C0A-46E2-42E4-B0CA-F2E6B1642311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E367C72-C3CD-4EA5-B90A-FC79D9C8C1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="79">
   <si>
     <t>iteration</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>N of plies 5th iteration</t>
+  </si>
+  <si>
+    <t>Average n of plies (i1-i4)</t>
   </si>
 </sst>
 </file>
@@ -9092,16 +9098,16 @@
   <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L47" sqref="L47:L55"/>
+      <selection pane="bottomRight" activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="3.75" customWidth="1"/>
-    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.25" customWidth="1"/>
     <col min="17" max="25" width="8.625" customWidth="1"/>
     <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -9977,43 +9983,43 @@
         <v>38</v>
       </c>
       <c r="P14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Q14" s="5">
-        <f>_xlfn.STDEV.S(Q6:Q10)</f>
-        <v>0.83666002653407556</v>
+        <f>AVERAGE(Q6:Q10)</f>
+        <v>155.80000000000001</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" ref="R14:Y14" si="0">_xlfn.STDEV.S(R6:R10)</f>
-        <v>0.54772255750516607</v>
+        <f t="shared" ref="R14:Y14" si="0">AVERAGE(R6:R10)</f>
+        <v>119.4</v>
       </c>
       <c r="S14" s="5">
         <f t="shared" si="0"/>
-        <v>1.2247448713915889</v>
+        <v>79</v>
       </c>
       <c r="T14" s="5">
         <f t="shared" si="0"/>
-        <v>1.0954451150103321</v>
+        <v>83.2</v>
       </c>
       <c r="U14" s="5">
         <f t="shared" si="0"/>
-        <v>0.44721359549995793</v>
+        <v>125.8</v>
       </c>
       <c r="V14" s="5">
         <f t="shared" si="0"/>
-        <v>1.3416407864998738</v>
+        <v>162.4</v>
       </c>
       <c r="W14" s="5">
         <f t="shared" si="0"/>
-        <v>0.83666002653407556</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="X14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="Y14" s="5">
         <f t="shared" si="0"/>
-        <v>1.0954451150103321</v>
+        <v>85.8</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -10056,6 +10062,36 @@
       <c r="M15" t="s">
         <v>38</v>
       </c>
+      <c r="P15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q15">
+        <v>156</v>
+      </c>
+      <c r="R15">
+        <v>119</v>
+      </c>
+      <c r="S15">
+        <v>79</v>
+      </c>
+      <c r="T15">
+        <v>82</v>
+      </c>
+      <c r="U15">
+        <v>126</v>
+      </c>
+      <c r="V15">
+        <v>163</v>
+      </c>
+      <c r="W15">
+        <v>164</v>
+      </c>
+      <c r="X15">
+        <v>124</v>
+      </c>
+      <c r="Y15">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -10096,6 +10132,45 @@
       </c>
       <c r="M16" t="s">
         <v>38</v>
+      </c>
+      <c r="P16" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>_xlfn.STDEV.P(Q6:Q10)</f>
+        <v>0.74833147735478833</v>
+      </c>
+      <c r="R16" s="5">
+        <f>_xlfn.STDEV.S(R6:R10)</f>
+        <v>0.54772255750516607</v>
+      </c>
+      <c r="S16" s="5">
+        <f>_xlfn.STDEV.S(S6:S10)</f>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="T16" s="5">
+        <f>_xlfn.STDEV.S(T6:T10)</f>
+        <v>1.0954451150103321</v>
+      </c>
+      <c r="U16" s="5">
+        <f>_xlfn.STDEV.S(U6:U10)</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="V16" s="5">
+        <f>_xlfn.STDEV.S(V6:V10)</f>
+        <v>1.3416407864998738</v>
+      </c>
+      <c r="W16" s="5">
+        <f>_xlfn.STDEV.S(W6:W10)</f>
+        <v>0.83666002653407556</v>
+      </c>
+      <c r="X16" s="5">
+        <f>_xlfn.STDEV.S(X6:X10)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="5">
+        <f>_xlfn.STDEV.S(Y6:Y10)</f>
+        <v>1.0954451150103321</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>